<commit_message>
Test output in E0
</commit_message>
<xml_diff>
--- a/reports/product_report.xlsx
+++ b/reports/product_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>No.</t>
   </si>
@@ -41,28 +41,10 @@
     <t>Total(Php)</t>
   </si>
   <si>
-    <t>AFICIONADO ASSTD 85ML</t>
-  </si>
-  <si>
-    <t>ITM105907</t>
-  </si>
-  <si>
-    <t>ZONROX COLORSAFE 225ML</t>
-  </si>
-  <si>
-    <t>ITM100812</t>
-  </si>
-  <si>
-    <t>ZONROX ORIGINAL 500ML</t>
-  </si>
-  <si>
-    <t>ITM100799</t>
-  </si>
-  <si>
-    <t>ZONROX COLORSAFE 900ML</t>
-  </si>
-  <si>
-    <t>ITM100810</t>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Supremo Beer 1L</t>
   </si>
 </sst>
 </file>
@@ -438,19 +420,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:H5"/>
+      <selection activeCell="A1" sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.856" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="29.279" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="6.856" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="15.139" bestFit="true" customWidth="true" style="0"/>
@@ -489,23 +471,23 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2">
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E2" s="2">
-        <v>238.0</v>
+        <v>130.0</v>
       </c>
       <c r="F2" s="2">
-        <v>58.93</v>
+        <v>49.92</v>
       </c>
       <c r="G2" s="2">
-        <v>275.0</v>
+        <v>208.0</v>
       </c>
       <c r="H2" s="2">
-        <v>262.73</v>
+        <v>374.4</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -513,77 +495,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="2">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" s="2">
-        <v>22.75</v>
+        <v>150.0</v>
       </c>
       <c r="F3" s="2">
-        <v>14.46</v>
+        <v>19.8</v>
       </c>
       <c r="G3" s="2">
-        <v>27.0</v>
+        <v>165.0</v>
       </c>
       <c r="H3" s="2">
-        <v>128.97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20.03</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2.68</v>
-      </c>
-      <c r="G4" s="2">
-        <v>25.0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>23.88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>63.0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>15.0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>133.75</v>
+        <v>156.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>